<commit_message>
correcoes devido a troca de nome dos arquivos
</commit_message>
<xml_diff>
--- a/phaser/no-boo/Planejamento.xlsx
+++ b/phaser/no-boo/Planejamento.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Planejamento do Projeto</t>
   </si>
@@ -40,30 +40,15 @@
     <t>07/02</t>
   </si>
   <si>
-    <t>Desenhar os sprites: fantasminhas, explosões e telas</t>
-  </si>
-  <si>
     <t>Estudar o Phaser</t>
   </si>
   <si>
-    <t>Colocar os sprites na tela</t>
-  </si>
-  <si>
-    <t>Colocar o som</t>
-  </si>
-  <si>
     <t>Anne</t>
   </si>
   <si>
     <t>Matheus</t>
   </si>
   <si>
-    <t>Fazer os movimentos dos fantasminhas: horizontal, vertical, diagonal</t>
-  </si>
-  <si>
-    <t>Trabalhar nos extras da tela de jogo: pontuação, vida, relógio</t>
-  </si>
-  <si>
     <t>Dar sentido ao tap: fantasminha = explosão; pac = brilho</t>
   </si>
   <si>
@@ -76,16 +61,37 @@
     <t>x</t>
   </si>
   <si>
-    <t>Desenhar as telas: splash, menu, instruções, créditos, de ganhar, de perder</t>
-  </si>
-  <si>
     <t>Baixar os sons: menu, fundo do jogo, quando apertar no pac, quando matar fantasma, quando ganhar, quando perder</t>
   </si>
   <si>
-    <t>Fazer a transição entre as telas: splash do grupo, splash do jogo, menu, créditos, jogo, ganhou/perdeu</t>
-  </si>
-  <si>
     <t>A FAZER</t>
+  </si>
+  <si>
+    <t>Trabalhar nos extras da tela de jogo: pontuação, vida, cronometro</t>
+  </si>
+  <si>
+    <t>Fazer os movimentos dos fantasminhas e dos pac's: horizontal, vertical, diagonal</t>
+  </si>
+  <si>
+    <t>Desenhar os sprites: fantasminhas, pac's, explosões e telas</t>
+  </si>
+  <si>
+    <t>Desenhar as telas: splash do jogo, menu, como jogar, créditos, ganhou, perdeu</t>
+  </si>
+  <si>
+    <t>Colocar um fantasminha na tela, como exemplo</t>
+  </si>
+  <si>
+    <t>Colocar um som no jogo, como exemplo</t>
+  </si>
+  <si>
+    <t>Fazer a transição entre as telas: splash do grupo, splash do jogo, menu, como jogar, créditos, jogo, ganhou/perdeu</t>
+  </si>
+  <si>
+    <t>Posicionar aleatoriamente x fantasminhas e y pac's ao iniciar o jogo</t>
+  </si>
+  <si>
+    <t>Juntar tudo</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -461,11 +467,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -539,6 +554,24 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,22 +602,11 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -888,7 +910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -902,13 +924,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -917,10 +939,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>2</v>
@@ -928,221 +950,229 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="15" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="16" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="17" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="28" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="40" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="44" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34" t="s">
+        <v>16</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="44"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="46"/>
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="B13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="34"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+    <row r="14" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+    <row r="16" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="42"/>
+      <c r="B17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39">
+      <c r="B19" s="44"/>
+      <c r="C19" s="45">
         <v>41677</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,15 +1223,31 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
+    <row r="27" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
refatoracao do codigo, complemento ao movimento do sprites, pontuacao, vidas
</commit_message>
<xml_diff>
--- a/phaser/no-boo/Planejamento.xlsx
+++ b/phaser/no-boo/Planejamento.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Planejamento do Projeto</t>
   </si>
@@ -102,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
     <numFmt numFmtId="165" formatCode="d\-mmm;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -189,6 +189,11 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -560,16 +565,14 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -602,11 +605,13 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1070,10 +1075,12 @@
       <c r="B11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34" t="s">
-        <v>16</v>
+      <c r="C11" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48" t="s">
+        <v>14</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -1082,10 +1089,12 @@
       <c r="B12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34" t="s">
-        <v>16</v>
+      <c r="C12" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48" t="s">
+        <v>14</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1094,11 +1103,11 @@
       <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="34"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="48"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1106,13 +1115,13 @@
       <c r="B14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="36"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="49" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1129,12 +1138,12 @@
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>